<commit_message>
bacterial growth template update
</commit_message>
<xml_diff>
--- a/templates/community/CEPLAS-data/bacterial_growth_conditions.xlsx
+++ b/templates/community/CEPLAS-data/bacterial_growth_conditions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_ori\Desktop\arcs\Swate-templates\templates\community\CEPLAS-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55291490-983A-43AB-9B60-A2460B2717BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D8DDC3-C9A2-4434-92EF-76186DC9F3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="1" xr2:uid="{247AEDDF-3CEC-4F1D-B996-6B655E69C0BC}"/>
+    <workbookView xWindow="5568" yWindow="2208" windowWidth="17280" windowHeight="8880" xr2:uid="{247AEDDF-3CEC-4F1D-B996-6B655E69C0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="77">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="94">
   <si>
     <t>Source Name</t>
   </si>
@@ -118,15 +118,6 @@
     <t>Term Accession Number (PATO:0000146)</t>
   </si>
   <si>
-    <t>Parameter [Agitation]</t>
-  </si>
-  <si>
-    <t>Term Source REF (NCIT:C79530)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (NCIT:C79530)</t>
-  </si>
-  <si>
     <t>Parameter [Light intensity]</t>
   </si>
   <si>
@@ -136,15 +127,6 @@
     <t>Term Accession Number (MIAPPE:0101)</t>
   </si>
   <si>
-    <t>Parameter [carbon dioxide]</t>
-  </si>
-  <si>
-    <t>Term Source REF (CHEBI:16526)</t>
-  </si>
-  <si>
-    <t>Term Accession Number (CHEBI:16526)</t>
-  </si>
-  <si>
     <t>Id</t>
   </si>
   <si>
@@ -266,12 +248,89 @@
   </si>
   <si>
     <t>culture conditions</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit  </t>
+  </si>
+  <si>
+    <t>Parameter [Shake]</t>
+  </si>
+  <si>
+    <t>Term Source REF (NCIT:C64646)</t>
+  </si>
+  <si>
+    <t>Term Accession Number (NCIT:C64646)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit   </t>
+  </si>
+  <si>
+    <t>milliliter</t>
+  </si>
+  <si>
+    <t>UO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000098</t>
+  </si>
+  <si>
+    <t>microgram per milliliter</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000274</t>
+  </si>
+  <si>
+    <t>degree celsius</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000027</t>
+  </si>
+  <si>
+    <t>microeinstein per square meter per second</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000160</t>
+  </si>
+  <si>
+    <t>Parameter [carbon dioxide concentration]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit    </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term Source REF ()     </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Term Accession Number ()     </t>
+  </si>
+  <si>
+    <t>percent</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/UO_0000187</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit     </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="6">
+    <numFmt numFmtId="164" formatCode="0.00\ &quot;milliliter&quot;"/>
+    <numFmt numFmtId="165" formatCode="0.00\ &quot;microgram per milliliter&quot;"/>
+    <numFmt numFmtId="166" formatCode="0.00\ &quot;degree celsius&quot;"/>
+    <numFmt numFmtId="167" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
+    <numFmt numFmtId="168" formatCode="0.00\ &quot;percent&quot;"/>
+    <numFmt numFmtId="169" formatCode="0.00\ &quot;hours&quot;"/>
+  </numFmts>
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -418,7 +477,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -451,41 +510,65 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="33">
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
+  <dxfs count="39">
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.00\ &quot;hours&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00\ &quot;percent&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="165" formatCode="0.00\ &quot;microgram per milliliter&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.00\ &quot;milliliter&quot;"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -570,43 +653,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A295E0E-BF6B-4346-BC18-6E25EA372EEA}" name="annotationTableShyLion39" displayName="annotationTableShyLion39" ref="A1:AI2" totalsRowShown="0">
-  <autoFilter ref="A1:AI2" xr:uid="{8A295E0E-BF6B-4346-BC18-6E25EA372EEA}"/>
-  <tableColumns count="35">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{8A295E0E-BF6B-4346-BC18-6E25EA372EEA}" name="annotationTableShyLion39" displayName="annotationTableShyLion39" ref="A1:AO2" totalsRowShown="0">
+  <autoFilter ref="A1:AO2" xr:uid="{8A295E0E-BF6B-4346-BC18-6E25EA372EEA}"/>
+  <tableColumns count="41">
     <tableColumn id="1" xr3:uid="{D186EFC6-5ABC-42C6-9232-BCFF34AE78A2}" name="Source Name"/>
-    <tableColumn id="6" xr3:uid="{FD6E2B11-1728-4FEF-A797-97A29E65176D}" name="Characteristic [organism]" dataDxfId="32"/>
-    <tableColumn id="7" xr3:uid="{63B80971-7018-4A6E-829F-C3269CBE8A53}" name="Term Source REF (OBI:0100026)" dataDxfId="31"/>
-    <tableColumn id="8" xr3:uid="{89B1ED8F-2B74-4C6B-B40F-A0CB14C246FB}" name="Term Accession Number (OBI:0100026)" dataDxfId="30"/>
-    <tableColumn id="9" xr3:uid="{124A80DB-CE3D-44DF-970A-C5CFAEED4293}" name="Parameter [inoculation medium]" dataDxfId="29"/>
-    <tableColumn id="10" xr3:uid="{B44636D0-FC77-4FF0-89D3-E3BC385B6C51}" name="Term Source REF ()" dataDxfId="28"/>
-    <tableColumn id="11" xr3:uid="{806F7C83-EFE2-44B2-AA84-DCCAE8888406}" name="Term Accession Number ()" dataDxfId="27"/>
-    <tableColumn id="12" xr3:uid="{B32F3CAC-B9D1-40B9-A6AD-E580F74504FA}" name="Parameter [inoculation medium volume]" dataDxfId="26"/>
-    <tableColumn id="13" xr3:uid="{7BCF0DD0-7A9E-4877-9DA0-0BD97EC535DF}" name="Term Source REF () " dataDxfId="25"/>
-    <tableColumn id="14" xr3:uid="{05502792-8207-494E-915C-4A83E2A8209C}" name="Term Accession Number () " dataDxfId="24"/>
-    <tableColumn id="15" xr3:uid="{32DB2464-BCDE-483E-AF08-8040A5260089}" name="Parameter [Antibiotic]" dataDxfId="23"/>
-    <tableColumn id="16" xr3:uid="{F8635FEF-78A9-45A6-80FE-8BF129D87A89}" name="Term Source REF (NCIT:C258)" dataDxfId="22"/>
-    <tableColumn id="17" xr3:uid="{E513D31C-96CF-4DF0-A108-DA23348487E6}" name="Term Accession Number (NCIT:C258)" dataDxfId="21"/>
-    <tableColumn id="18" xr3:uid="{915DA3C3-4AF6-4ED6-8A8B-26F5AA513F0C}" name="Parameter [Antibiotic volume]" dataDxfId="20"/>
-    <tableColumn id="19" xr3:uid="{DD06E0EA-E13A-43BF-80AC-ABAADC8F233E}" name="Term Source REF ()  " dataDxfId="19"/>
-    <tableColumn id="20" xr3:uid="{4F6AAA21-CDA5-4BCB-9216-76C78AD588C5}" name="Term Accession Number ()  " dataDxfId="18"/>
-    <tableColumn id="21" xr3:uid="{C4FD6D55-C7A5-42CC-ACE8-B4F12711B936}" name="Parameter [OD750]" dataDxfId="17"/>
-    <tableColumn id="22" xr3:uid="{72557795-0E6F-431E-B308-3B95C538FAC1}" name="Term Source REF ()   " dataDxfId="16"/>
-    <tableColumn id="23" xr3:uid="{87D447FF-8544-443D-A574-E93F51A57EF0}" name="Term Accession Number ()   " dataDxfId="15"/>
-    <tableColumn id="27" xr3:uid="{944B63CE-5295-424D-A5DA-8C3560F37A77}" name="Parameter [growth time]" dataDxfId="14"/>
-    <tableColumn id="28" xr3:uid="{4FDEBA05-3F9B-4F34-ACFA-2FA23210F924}" name="Term Source REF ()    " dataDxfId="13"/>
-    <tableColumn id="29" xr3:uid="{8A089780-7967-41E6-AF75-EC401AC624CE}" name="Term Accession Number ()    " dataDxfId="12"/>
+    <tableColumn id="6" xr3:uid="{FD6E2B11-1728-4FEF-A797-97A29E65176D}" name="Characteristic [organism]" dataDxfId="38"/>
+    <tableColumn id="7" xr3:uid="{63B80971-7018-4A6E-829F-C3269CBE8A53}" name="Term Source REF (OBI:0100026)" dataDxfId="37"/>
+    <tableColumn id="8" xr3:uid="{89B1ED8F-2B74-4C6B-B40F-A0CB14C246FB}" name="Term Accession Number (OBI:0100026)" dataDxfId="36"/>
+    <tableColumn id="9" xr3:uid="{124A80DB-CE3D-44DF-970A-C5CFAEED4293}" name="Parameter [inoculation medium]" dataDxfId="35"/>
+    <tableColumn id="10" xr3:uid="{B44636D0-FC77-4FF0-89D3-E3BC385B6C51}" name="Term Source REF ()" dataDxfId="34"/>
+    <tableColumn id="11" xr3:uid="{806F7C83-EFE2-44B2-AA84-DCCAE8888406}" name="Term Accession Number ()" dataDxfId="33"/>
+    <tableColumn id="12" xr3:uid="{B32F3CAC-B9D1-40B9-A6AD-E580F74504FA}" name="Parameter [inoculation medium volume]" dataDxfId="15"/>
+    <tableColumn id="3" xr3:uid="{792731F0-9849-49AD-9B82-2550DA0DFF16}" name="Unit" dataDxfId="16"/>
+    <tableColumn id="13" xr3:uid="{7BCF0DD0-7A9E-4877-9DA0-0BD97EC535DF}" name="Term Source REF () " dataDxfId="32"/>
+    <tableColumn id="14" xr3:uid="{05502792-8207-494E-915C-4A83E2A8209C}" name="Term Accession Number () " dataDxfId="31"/>
+    <tableColumn id="15" xr3:uid="{32DB2464-BCDE-483E-AF08-8040A5260089}" name="Parameter [Antibiotic]" dataDxfId="30"/>
+    <tableColumn id="16" xr3:uid="{F8635FEF-78A9-45A6-80FE-8BF129D87A89}" name="Term Source REF (NCIT:C258)" dataDxfId="29"/>
+    <tableColumn id="17" xr3:uid="{E513D31C-96CF-4DF0-A108-DA23348487E6}" name="Term Accession Number (NCIT:C258)" dataDxfId="28"/>
+    <tableColumn id="18" xr3:uid="{915DA3C3-4AF6-4ED6-8A8B-26F5AA513F0C}" name="Parameter [Antibiotic volume]" dataDxfId="13"/>
+    <tableColumn id="4" xr3:uid="{E75F9782-FB52-4626-B223-4A5FB26B14C9}" name="Unit " dataDxfId="14"/>
+    <tableColumn id="19" xr3:uid="{DD06E0EA-E13A-43BF-80AC-ABAADC8F233E}" name="Term Source REF ()  " dataDxfId="27"/>
+    <tableColumn id="20" xr3:uid="{4F6AAA21-CDA5-4BCB-9216-76C78AD588C5}" name="Term Accession Number ()  " dataDxfId="26"/>
+    <tableColumn id="21" xr3:uid="{C4FD6D55-C7A5-42CC-ACE8-B4F12711B936}" name="Parameter [OD750]" dataDxfId="25"/>
+    <tableColumn id="22" xr3:uid="{72557795-0E6F-431E-B308-3B95C538FAC1}" name="Term Source REF ()   " dataDxfId="24"/>
+    <tableColumn id="23" xr3:uid="{87D447FF-8544-443D-A574-E93F51A57EF0}" name="Term Accession Number ()   " dataDxfId="23"/>
+    <tableColumn id="27" xr3:uid="{944B63CE-5295-424D-A5DA-8C3560F37A77}" name="Parameter [growth time]" dataDxfId="0"/>
+    <tableColumn id="38" xr3:uid="{5234BA64-B6B9-4855-A887-ACCBC2DCCF60}" name="Unit     " dataDxfId="1"/>
+    <tableColumn id="28" xr3:uid="{4FDEBA05-3F9B-4F34-ACFA-2FA23210F924}" name="Term Source REF ()    " dataDxfId="22"/>
+    <tableColumn id="29" xr3:uid="{8A089780-7967-41E6-AF75-EC401AC624CE}" name="Term Accession Number ()    " dataDxfId="21"/>
     <tableColumn id="30" xr3:uid="{F72DBE16-8C7C-427C-B5EE-567E9E536C64}" name="Parameter [temperature]" dataDxfId="11"/>
-    <tableColumn id="31" xr3:uid="{30BCC5B6-4EDD-40CB-ACD9-94DD10EF5327}" name="Term Source REF (PATO:0000146)" dataDxfId="10"/>
-    <tableColumn id="32" xr3:uid="{92E7C17F-DD20-4675-B0F0-DA6B586F40AA}" name="Term Accession Number (PATO:0000146)" dataDxfId="9"/>
-    <tableColumn id="36" xr3:uid="{95E44477-438D-49B8-95FF-63D7E9EC45EC}" name="Parameter [Agitation]" dataDxfId="8"/>
-    <tableColumn id="37" xr3:uid="{A7EF9D6F-C9EB-419E-AE63-96B4D3D36170}" name="Term Source REF (NCIT:C79530)" dataDxfId="7"/>
-    <tableColumn id="38" xr3:uid="{C17420F0-C3FC-4E9B-8B7E-BD53F570C311}" name="Term Accession Number (NCIT:C79530)" dataDxfId="6"/>
-    <tableColumn id="39" xr3:uid="{2A6F761F-8379-4E4B-9273-4FEF8CF2366A}" name="Parameter [Light intensity]" dataDxfId="5"/>
-    <tableColumn id="40" xr3:uid="{9B26BD22-901D-40CE-991A-38D82DD6AFA2}" name="Term Source REF (MIAPPE:0101)" dataDxfId="4"/>
-    <tableColumn id="41" xr3:uid="{1045AE36-88A1-4A78-BF95-4332581DAE4E}" name="Term Accession Number (MIAPPE:0101)" dataDxfId="3"/>
-    <tableColumn id="42" xr3:uid="{2EFF7398-A6DB-4E45-B8CF-8177588CDD47}" name="Parameter [carbon dioxide]" dataDxfId="2"/>
-    <tableColumn id="43" xr3:uid="{5CA0D78F-2789-4BF6-ABF9-314CE3128928}" name="Term Source REF (CHEBI:16526)" dataDxfId="1"/>
-    <tableColumn id="44" xr3:uid="{E549F61C-DC19-4A0C-8968-B767C328AE49}" name="Term Accession Number (CHEBI:16526)" dataDxfId="0"/>
+    <tableColumn id="5" xr3:uid="{B3A979FF-58B0-4979-A959-CC2954224133}" name="Unit  " dataDxfId="12"/>
+    <tableColumn id="31" xr3:uid="{30BCC5B6-4EDD-40CB-ACD9-94DD10EF5327}" name="Term Source REF (PATO:0000146)" dataDxfId="20"/>
+    <tableColumn id="32" xr3:uid="{92E7C17F-DD20-4675-B0F0-DA6B586F40AA}" name="Term Accession Number (PATO:0000146)" dataDxfId="19"/>
+    <tableColumn id="24" xr3:uid="{92CEB919-B207-4A93-88A2-A9B74768E523}" name="Parameter [Shake]" dataDxfId="10"/>
+    <tableColumn id="25" xr3:uid="{38AF0F25-7FA8-4A6A-B29E-872521A63937}" name="Term Source REF (NCIT:C64646)" dataDxfId="9"/>
+    <tableColumn id="26" xr3:uid="{850074F3-B805-43AD-A2B5-D001C3D127B0}" name="Term Accession Number (NCIT:C64646)" dataDxfId="8"/>
+    <tableColumn id="39" xr3:uid="{2A6F761F-8379-4E4B-9273-4FEF8CF2366A}" name="Parameter [Light intensity]" dataDxfId="6"/>
+    <tableColumn id="33" xr3:uid="{E17A20CF-CC57-483F-85FD-DE6D0F712E3B}" name="Unit   " dataDxfId="7"/>
+    <tableColumn id="40" xr3:uid="{9B26BD22-901D-40CE-991A-38D82DD6AFA2}" name="Term Source REF (MIAPPE:0101)" dataDxfId="18"/>
+    <tableColumn id="41" xr3:uid="{1045AE36-88A1-4A78-BF95-4332581DAE4E}" name="Term Accession Number (MIAPPE:0101)" dataDxfId="17"/>
+    <tableColumn id="34" xr3:uid="{2B38AFCE-C973-4A32-B262-F5A8C1EA5B0E}" name="Parameter [carbon dioxide concentration]" dataDxfId="5"/>
+    <tableColumn id="35" xr3:uid="{1333A948-5C00-4DAF-BE65-21B9503A89A3}" name="Unit    " dataDxfId="4"/>
+    <tableColumn id="36" xr3:uid="{3000F4B5-285D-41EB-999D-A4B47E758A95}" name="Term Source REF ()     " dataDxfId="3"/>
+    <tableColumn id="37" xr3:uid="{66544E85-0AA3-4BB8-A26A-32A374635904}" name="Term Accession Number ()     " dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{98899D0F-E7C8-4D35-9E8F-8B4EE59AE0DB}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -910,7 +999,7 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="438" row="0">
+  <wetp:taskpane dockstate="right" visibility="0" width="574" row="0">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
   <wetp:taskpane dockstate="right" visibility="0" width="438" row="0">
@@ -941,9 +1030,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92717983-C2E7-4C02-964F-184C0402CA6A}">
-  <dimension ref="A1:AI2"/>
+  <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V1" sqref="V1:V1048576"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -955,36 +1046,41 @@
     <col min="6" max="6" width="19.109375" hidden="1" customWidth="1"/>
     <col min="7" max="7" width="25.6640625" hidden="1" customWidth="1"/>
     <col min="8" max="8" width="38.109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.6640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="26.109375" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="22.109375" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="28.109375" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="34.5546875" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="29.109375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="20.109375" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="26.5546875" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="19.5546875" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.5546875" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="27" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="27.44140625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="24.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="31.77734375" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="38.21875" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="30.109375" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="36.6640625" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="30.77734375" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="26.5546875" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="30" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="36.5546875" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5546875" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="19.6640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="37.88671875" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="22.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="28.109375" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="34.5546875" hidden="1" customWidth="1"/>
+    <col min="15" max="15" width="29.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="20.109375" hidden="1" customWidth="1"/>
+    <col min="18" max="18" width="37.88671875" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="19.5546875" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="20.5546875" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="27" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="21" hidden="1" customWidth="1"/>
+    <col min="24" max="24" width="27.44140625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="24.6640625" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="24.6640625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="31.77734375" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="38.21875" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="19" hidden="1" customWidth="1"/>
+    <col min="30" max="30" width="19" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="36.6640625" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="25.88671875" hidden="1" customWidth="1"/>
+    <col min="33" max="33" width="25.88671875" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="30.77734375" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="37.88671875" hidden="1" customWidth="1"/>
+    <col min="36" max="36" width="39.109375" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="39.109375" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="21.44140625" hidden="1" customWidth="1"/>
+    <col min="39" max="39" width="28" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="14.88671875" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="14.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1010,88 +1106,106 @@
         <v>9</v>
       </c>
       <c r="I1" t="s">
+        <v>71</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>14</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>15</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
+        <v>72</v>
+      </c>
+      <c r="Q1" t="s">
         <v>16</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>17</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="S1" t="s">
         <v>18</v>
       </c>
-      <c r="R1" t="s">
+      <c r="T1" t="s">
         <v>19</v>
       </c>
-      <c r="S1" t="s">
+      <c r="U1" t="s">
         <v>20</v>
       </c>
-      <c r="T1" t="s">
+      <c r="V1" t="s">
         <v>21</v>
       </c>
-      <c r="U1" t="s">
+      <c r="W1" t="s">
+        <v>93</v>
+      </c>
+      <c r="X1" t="s">
         <v>22</v>
       </c>
-      <c r="V1" t="s">
+      <c r="Y1" t="s">
         <v>23</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Z1" t="s">
         <v>24</v>
       </c>
-      <c r="X1" t="s">
+      <c r="AA1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB1" t="s">
         <v>25</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AC1" t="s">
         <v>26</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AD1" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>75</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AG1" t="s">
         <v>27</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AH1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AI1" t="s">
         <v>28</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AJ1" t="s">
         <v>29</v>
       </c>
-      <c r="AC1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AI1" t="s">
+      <c r="AK1" t="s">
+        <v>87</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>88</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>89</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>90</v>
+      </c>
+      <c r="AO1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" x14ac:dyDescent="0.3">
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
         <v>3</v>
@@ -1108,17 +1222,17 @@
       <c r="G2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="H2" s="1" t="s">
+      <c r="H2" s="12" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>3</v>
+        <v>78</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>3</v>
+        <v>80</v>
       </c>
       <c r="L2" s="1" t="s">
         <v>3</v>
@@ -1129,17 +1243,17 @@
       <c r="N2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="O2" s="13" t="s">
         <v>3</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>3</v>
+        <v>81</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>3</v>
+        <v>82</v>
       </c>
       <c r="S2" s="1" t="s">
         <v>3</v>
@@ -1150,29 +1264,27 @@
       <c r="U2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="V2" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="W2" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="V2" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="W2" s="1"/>
       <c r="X2" s="1" t="s">
         <v>3</v>
       </c>
       <c r="Y2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="Z2" s="14" t="s">
         <v>3</v>
       </c>
       <c r="AA2" s="1" t="s">
-        <v>3</v>
+        <v>83</v>
       </c>
       <c r="AB2" s="1" t="s">
-        <v>3</v>
+        <v>79</v>
       </c>
       <c r="AC2" s="1" t="s">
-        <v>3</v>
+        <v>84</v>
       </c>
       <c r="AD2" s="1" t="s">
         <v>3</v>
@@ -1183,11 +1295,29 @@
       <c r="AF2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="AG2" s="1" t="s">
+      <c r="AG2" s="15" t="s">
         <v>3</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>3</v>
+        <v>85</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AJ2" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AK2" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="AL2" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="AM2" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN2" s="1" t="s">
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -1202,7 +1332,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1ED65C-31D9-4AD3-B87A-AB0F34D6753A}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
@@ -1213,79 +1343,79 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B1" s="10" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="B7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
       <c r="B8" s="7"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="B10" s="3"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -1293,119 +1423,119 @@
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
-        <v>47</v>
+        <v>41</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D12" s="7" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C13" s="3"/>
       <c r="D13" s="3"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C14" s="3"/>
       <c r="D14" s="3"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="B15" s="6"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="B18" s="3"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>54</v>
+        <v>48</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20" s="4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="B20" s="3"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="B21" s="3"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="B22" s="3"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23" s="4" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="B23" s="3"/>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24" s="4" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="B24" s="3"/>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25" s="4" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="B25" s="3"/>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26" s="4" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="B26" s="3"/>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="8" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
       <c r="B27" s="9"/>
     </row>

</xml_diff>

<commit_message>
change metadata sheet to isa template
</commit_message>
<xml_diff>
--- a/templates/community/CEPLAS-data/bacterial_growth_conditions.xlsx
+++ b/templates/community/CEPLAS-data/bacterial_growth_conditions.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t_ori\Desktop\arcs\Swate-templates\templates\community\CEPLAS-data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stella Eggels\Documents\GitHub\Swate-templates\templates\community\CEPLAS-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87D8DDC3-C9A2-4434-92EF-76186DC9F3B3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95C9BD0-8934-4596-AAB0-172FD1AEFFAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5568" yWindow="2208" windowWidth="17280" windowHeight="8880" xr2:uid="{247AEDDF-3CEC-4F1D-B996-6B655E69C0BC}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{247AEDDF-3CEC-4F1D-B996-6B655E69C0BC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="SwateTemplateMetadata" sheetId="2" r:id="rId2"/>
+    <sheet name="isa_template" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -518,11 +518,65 @@
     <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Link" xfId="1" builtinId="8"/>
+    <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="39">
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="168" formatCode="0.00\ &quot;percent&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="167" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree celsius&quot;"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="169" formatCode="0.00\ &quot;hours&quot;"/>
     </dxf>
     <dxf>
@@ -538,25 +592,7 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="168" formatCode="0.00\ &quot;percent&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="167" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="166" formatCode="0.00\ &quot;degree celsius&quot;"/>
+      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -568,58 +604,22 @@
       <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;milliliter&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="30" formatCode="@"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="30" formatCode="@"/>
@@ -663,39 +663,39 @@
     <tableColumn id="9" xr3:uid="{124A80DB-CE3D-44DF-970A-C5CFAEED4293}" name="Parameter [inoculation medium]" dataDxfId="35"/>
     <tableColumn id="10" xr3:uid="{B44636D0-FC77-4FF0-89D3-E3BC385B6C51}" name="Term Source REF ()" dataDxfId="34"/>
     <tableColumn id="11" xr3:uid="{806F7C83-EFE2-44B2-AA84-DCCAE8888406}" name="Term Accession Number ()" dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{B32F3CAC-B9D1-40B9-A6AD-E580F74504FA}" name="Parameter [inoculation medium volume]" dataDxfId="15"/>
-    <tableColumn id="3" xr3:uid="{792731F0-9849-49AD-9B82-2550DA0DFF16}" name="Unit" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{7BCF0DD0-7A9E-4877-9DA0-0BD97EC535DF}" name="Term Source REF () " dataDxfId="32"/>
-    <tableColumn id="14" xr3:uid="{05502792-8207-494E-915C-4A83E2A8209C}" name="Term Accession Number () " dataDxfId="31"/>
-    <tableColumn id="15" xr3:uid="{32DB2464-BCDE-483E-AF08-8040A5260089}" name="Parameter [Antibiotic]" dataDxfId="30"/>
-    <tableColumn id="16" xr3:uid="{F8635FEF-78A9-45A6-80FE-8BF129D87A89}" name="Term Source REF (NCIT:C258)" dataDxfId="29"/>
-    <tableColumn id="17" xr3:uid="{E513D31C-96CF-4DF0-A108-DA23348487E6}" name="Term Accession Number (NCIT:C258)" dataDxfId="28"/>
-    <tableColumn id="18" xr3:uid="{915DA3C3-4AF6-4ED6-8A8B-26F5AA513F0C}" name="Parameter [Antibiotic volume]" dataDxfId="13"/>
-    <tableColumn id="4" xr3:uid="{E75F9782-FB52-4626-B223-4A5FB26B14C9}" name="Unit " dataDxfId="14"/>
-    <tableColumn id="19" xr3:uid="{DD06E0EA-E13A-43BF-80AC-ABAADC8F233E}" name="Term Source REF ()  " dataDxfId="27"/>
-    <tableColumn id="20" xr3:uid="{4F6AAA21-CDA5-4BCB-9216-76C78AD588C5}" name="Term Accession Number ()  " dataDxfId="26"/>
-    <tableColumn id="21" xr3:uid="{C4FD6D55-C7A5-42CC-ACE8-B4F12711B936}" name="Parameter [OD750]" dataDxfId="25"/>
-    <tableColumn id="22" xr3:uid="{72557795-0E6F-431E-B308-3B95C538FAC1}" name="Term Source REF ()   " dataDxfId="24"/>
-    <tableColumn id="23" xr3:uid="{87D447FF-8544-443D-A574-E93F51A57EF0}" name="Term Accession Number ()   " dataDxfId="23"/>
-    <tableColumn id="27" xr3:uid="{944B63CE-5295-424D-A5DA-8C3560F37A77}" name="Parameter [growth time]" dataDxfId="0"/>
-    <tableColumn id="38" xr3:uid="{5234BA64-B6B9-4855-A887-ACCBC2DCCF60}" name="Unit     " dataDxfId="1"/>
-    <tableColumn id="28" xr3:uid="{4FDEBA05-3F9B-4F34-ACFA-2FA23210F924}" name="Term Source REF ()    " dataDxfId="22"/>
-    <tableColumn id="29" xr3:uid="{8A089780-7967-41E6-AF75-EC401AC624CE}" name="Term Accession Number ()    " dataDxfId="21"/>
-    <tableColumn id="30" xr3:uid="{F72DBE16-8C7C-427C-B5EE-567E9E536C64}" name="Parameter [temperature]" dataDxfId="11"/>
-    <tableColumn id="5" xr3:uid="{B3A979FF-58B0-4979-A959-CC2954224133}" name="Unit  " dataDxfId="12"/>
-    <tableColumn id="31" xr3:uid="{30BCC5B6-4EDD-40CB-ACD9-94DD10EF5327}" name="Term Source REF (PATO:0000146)" dataDxfId="20"/>
-    <tableColumn id="32" xr3:uid="{92E7C17F-DD20-4675-B0F0-DA6B586F40AA}" name="Term Accession Number (PATO:0000146)" dataDxfId="19"/>
+    <tableColumn id="12" xr3:uid="{B32F3CAC-B9D1-40B9-A6AD-E580F74504FA}" name="Parameter [inoculation medium volume]" dataDxfId="32"/>
+    <tableColumn id="3" xr3:uid="{792731F0-9849-49AD-9B82-2550DA0DFF16}" name="Unit" dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{7BCF0DD0-7A9E-4877-9DA0-0BD97EC535DF}" name="Term Source REF () " dataDxfId="30"/>
+    <tableColumn id="14" xr3:uid="{05502792-8207-494E-915C-4A83E2A8209C}" name="Term Accession Number () " dataDxfId="29"/>
+    <tableColumn id="15" xr3:uid="{32DB2464-BCDE-483E-AF08-8040A5260089}" name="Parameter [Antibiotic]" dataDxfId="28"/>
+    <tableColumn id="16" xr3:uid="{F8635FEF-78A9-45A6-80FE-8BF129D87A89}" name="Term Source REF (NCIT:C258)" dataDxfId="27"/>
+    <tableColumn id="17" xr3:uid="{E513D31C-96CF-4DF0-A108-DA23348487E6}" name="Term Accession Number (NCIT:C258)" dataDxfId="26"/>
+    <tableColumn id="18" xr3:uid="{915DA3C3-4AF6-4ED6-8A8B-26F5AA513F0C}" name="Parameter [Antibiotic volume]" dataDxfId="25"/>
+    <tableColumn id="4" xr3:uid="{E75F9782-FB52-4626-B223-4A5FB26B14C9}" name="Unit " dataDxfId="24"/>
+    <tableColumn id="19" xr3:uid="{DD06E0EA-E13A-43BF-80AC-ABAADC8F233E}" name="Term Source REF ()  " dataDxfId="23"/>
+    <tableColumn id="20" xr3:uid="{4F6AAA21-CDA5-4BCB-9216-76C78AD588C5}" name="Term Accession Number ()  " dataDxfId="22"/>
+    <tableColumn id="21" xr3:uid="{C4FD6D55-C7A5-42CC-ACE8-B4F12711B936}" name="Parameter [OD750]" dataDxfId="21"/>
+    <tableColumn id="22" xr3:uid="{72557795-0E6F-431E-B308-3B95C538FAC1}" name="Term Source REF ()   " dataDxfId="20"/>
+    <tableColumn id="23" xr3:uid="{87D447FF-8544-443D-A574-E93F51A57EF0}" name="Term Accession Number ()   " dataDxfId="19"/>
+    <tableColumn id="27" xr3:uid="{944B63CE-5295-424D-A5DA-8C3560F37A77}" name="Parameter [growth time]" dataDxfId="18"/>
+    <tableColumn id="38" xr3:uid="{5234BA64-B6B9-4855-A887-ACCBC2DCCF60}" name="Unit     " dataDxfId="17"/>
+    <tableColumn id="28" xr3:uid="{4FDEBA05-3F9B-4F34-ACFA-2FA23210F924}" name="Term Source REF ()    " dataDxfId="16"/>
+    <tableColumn id="29" xr3:uid="{8A089780-7967-41E6-AF75-EC401AC624CE}" name="Term Accession Number ()    " dataDxfId="15"/>
+    <tableColumn id="30" xr3:uid="{F72DBE16-8C7C-427C-B5EE-567E9E536C64}" name="Parameter [temperature]" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{B3A979FF-58B0-4979-A959-CC2954224133}" name="Unit  " dataDxfId="13"/>
+    <tableColumn id="31" xr3:uid="{30BCC5B6-4EDD-40CB-ACD9-94DD10EF5327}" name="Term Source REF (PATO:0000146)" dataDxfId="12"/>
+    <tableColumn id="32" xr3:uid="{92E7C17F-DD20-4675-B0F0-DA6B586F40AA}" name="Term Accession Number (PATO:0000146)" dataDxfId="11"/>
     <tableColumn id="24" xr3:uid="{92CEB919-B207-4A93-88A2-A9B74768E523}" name="Parameter [Shake]" dataDxfId="10"/>
     <tableColumn id="25" xr3:uid="{38AF0F25-7FA8-4A6A-B29E-872521A63937}" name="Term Source REF (NCIT:C64646)" dataDxfId="9"/>
     <tableColumn id="26" xr3:uid="{850074F3-B805-43AD-A2B5-D001C3D127B0}" name="Term Accession Number (NCIT:C64646)" dataDxfId="8"/>
-    <tableColumn id="39" xr3:uid="{2A6F761F-8379-4E4B-9273-4FEF8CF2366A}" name="Parameter [Light intensity]" dataDxfId="6"/>
-    <tableColumn id="33" xr3:uid="{E17A20CF-CC57-483F-85FD-DE6D0F712E3B}" name="Unit   " dataDxfId="7"/>
-    <tableColumn id="40" xr3:uid="{9B26BD22-901D-40CE-991A-38D82DD6AFA2}" name="Term Source REF (MIAPPE:0101)" dataDxfId="18"/>
-    <tableColumn id="41" xr3:uid="{1045AE36-88A1-4A78-BF95-4332581DAE4E}" name="Term Accession Number (MIAPPE:0101)" dataDxfId="17"/>
-    <tableColumn id="34" xr3:uid="{2B38AFCE-C973-4A32-B262-F5A8C1EA5B0E}" name="Parameter [carbon dioxide concentration]" dataDxfId="5"/>
-    <tableColumn id="35" xr3:uid="{1333A948-5C00-4DAF-BE65-21B9503A89A3}" name="Unit    " dataDxfId="4"/>
-    <tableColumn id="36" xr3:uid="{3000F4B5-285D-41EB-999D-A4B47E758A95}" name="Term Source REF ()     " dataDxfId="3"/>
-    <tableColumn id="37" xr3:uid="{66544E85-0AA3-4BB8-A26A-32A374635904}" name="Term Accession Number ()     " dataDxfId="2"/>
+    <tableColumn id="39" xr3:uid="{2A6F761F-8379-4E4B-9273-4FEF8CF2366A}" name="Parameter [Light intensity]" dataDxfId="7"/>
+    <tableColumn id="33" xr3:uid="{E17A20CF-CC57-483F-85FD-DE6D0F712E3B}" name="Unit   " dataDxfId="6"/>
+    <tableColumn id="40" xr3:uid="{9B26BD22-901D-40CE-991A-38D82DD6AFA2}" name="Term Source REF (MIAPPE:0101)" dataDxfId="5"/>
+    <tableColumn id="41" xr3:uid="{1045AE36-88A1-4A78-BF95-4332581DAE4E}" name="Term Accession Number (MIAPPE:0101)" dataDxfId="4"/>
+    <tableColumn id="34" xr3:uid="{2B38AFCE-C973-4A32-B262-F5A8C1EA5B0E}" name="Parameter [carbon dioxide concentration]" dataDxfId="3"/>
+    <tableColumn id="35" xr3:uid="{1333A948-5C00-4DAF-BE65-21B9503A89A3}" name="Unit    " dataDxfId="2"/>
+    <tableColumn id="36" xr3:uid="{3000F4B5-285D-41EB-999D-A4B47E758A95}" name="Term Source REF ()     " dataDxfId="1"/>
+    <tableColumn id="37" xr3:uid="{66544E85-0AA3-4BB8-A26A-32A374635904}" name="Term Accession Number ()     " dataDxfId="0"/>
     <tableColumn id="2" xr3:uid="{98899D0F-E7C8-4D35-9E8F-8B4EE59AE0DB}" name="Sample Name"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -703,9 +703,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -743,7 +743,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -849,7 +849,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -991,7 +991,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1032,11 +1032,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92717983-C2E7-4C02-964F-184C0402CA6A}">
   <dimension ref="A1:AO2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="V1" sqref="V1:V1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="24.44140625" bestFit="1" customWidth="1"/>
@@ -1332,11 +1332,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4A1ED65C-31D9-4AD3-B87A-AB0F34D6753A}">
   <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="32.109375" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>